<commit_message>
Rubrica de evaluación actualizada en 3/4/2025
Buena participación :)
</commit_message>
<xml_diff>
--- a/Rúbrica de Evaluación.xlsx
+++ b/Rúbrica de Evaluación.xlsx
@@ -1,25 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D719F057-915D-4804-9823-2A1DCBE6F73C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="24000" windowHeight="9480"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -27,6 +18,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,77 +29,413 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
+    <t>Calidad de Trabajo 25%</t>
+  </si>
+  <si>
+    <t>Puntualidad 25%</t>
+  </si>
+  <si>
+    <t>Participación 25%</t>
+  </si>
+  <si>
+    <t>Asistencia en la defensa 25%</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Observación</t>
+  </si>
+  <si>
     <t>Carlos Flores</t>
   </si>
   <si>
+    <t>No mostró algún avance de programación más que realizar la caja negra y aportar aspectos de KanBan</t>
+  </si>
+  <si>
     <t>Byron Rivera</t>
   </si>
   <si>
+    <t>Apoyó bastante al grupo con el plan de Cristian, todos en un módulo</t>
+  </si>
+  <si>
+    <t>Cristian Martínez</t>
+  </si>
+  <si>
+    <t>Dejó de avanzar cuando fue encargado colaborar con la parte de reporte de supervisor, se desconoce algún progreso por las validaciones más que el del teclado Enter, tuvo un momento para conversar respecto a correcciones</t>
+  </si>
+  <si>
     <t>Francisco Lozano</t>
   </si>
   <si>
-    <t>Cristian Martínez</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Observación</t>
-  </si>
-  <si>
-    <t>Calidad de Trabajo 25%</t>
-  </si>
-  <si>
-    <t>Puntualidad 25%</t>
-  </si>
-  <si>
-    <t>Participación 25%</t>
-  </si>
-  <si>
-    <t>Asistencia en la defensa 25%</t>
-  </si>
-  <si>
-    <t>Apoyó bastante al grupo con el plan de Cristian, todos en un módulo</t>
-  </si>
-  <si>
     <t>No mostró algún avance, y realizó poca participación</t>
-  </si>
-  <si>
-    <t>No mostró algún avance de programación más que realizar la caja negra y aportar aspectos de KanBan</t>
-  </si>
-  <si>
-    <t>Dejó de avanzar cuando fue encargado colaborar con la parte de reporte de supervisor, se desconoce algún progreso por las validaciones más que el del teclado Enter, tuvo un momento para conversar respecto a correcciones</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* \-??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -114,33 +443,316 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Coma" xfId="1" builtinId="3"/>
+    <cellStyle name="Moneda" xfId="2" builtinId="4"/>
+    <cellStyle name="Porcentaje" xfId="3" builtinId="5"/>
+    <cellStyle name="Coma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Moneda [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hipervínculo" xfId="6" builtinId="8"/>
+    <cellStyle name="Hipervínculo visitado" xfId="7" builtinId="9"/>
+    <cellStyle name="Nota" xfId="8" builtinId="10"/>
+    <cellStyle name="Texto de advertencia" xfId="9" builtinId="11"/>
+    <cellStyle name="Título" xfId="10" builtinId="15"/>
+    <cellStyle name="Texto explicativo" xfId="11" builtinId="53"/>
+    <cellStyle name="Título 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Título 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Título 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Título 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Entrada" xfId="16" builtinId="20"/>
+    <cellStyle name="Salida" xfId="17" builtinId="21"/>
+    <cellStyle name="Cálculo" xfId="18" builtinId="22"/>
+    <cellStyle name="Celda de comprobación" xfId="19" builtinId="23"/>
+    <cellStyle name="Celda vinculada" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Correcto" xfId="22" builtinId="26"/>
+    <cellStyle name="Incorrecto" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutro" xfId="24" builtinId="28"/>
+    <cellStyle name="Énfasis1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Énfasis1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Énfasis1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Énfasis1" xfId="28" builtinId="32"/>
+    <cellStyle name="Énfasis2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Énfasis2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Énfasis2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Énfasis2" xfId="32" builtinId="36"/>
+    <cellStyle name="Énfasis3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Énfasis3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Énfasis3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Énfasis3" xfId="36" builtinId="40"/>
+    <cellStyle name="Énfasis4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Énfasis4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Énfasis4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Énfasis4" xfId="40" builtinId="44"/>
+    <cellStyle name="Énfasis5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Énfasis5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Énfasis5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Énfasis5" xfId="44" builtinId="48"/>
+    <cellStyle name="Énfasis6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Énfasis6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Énfasis6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Énfasis6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -189,7 +801,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -222,26 +834,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -274,23 +869,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office 2013 - 2022">
@@ -432,45 +1010,40 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="C3:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelRow="6"/>
   <cols>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="17.4285714285714" customWidth="1"/>
+    <col min="5" max="5" width="11.7142857142857" customWidth="1"/>
+    <col min="6" max="6" width="12.4285714285714" customWidth="1"/>
+    <col min="8" max="8" width="15.1428571428571" customWidth="1"/>
+    <col min="9" max="9" width="19.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" ht="60" spans="4:9">
       <c r="D3" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H3" t="s">
         <v>4</v>
@@ -479,9 +1052,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="3:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" ht="90" spans="3:9">
       <c r="C4" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D4" s="2">
         <v>0.2</v>
@@ -499,13 +1072,13 @@
         <f>(SUM(D4:G4))</f>
         <v>0.91</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>12</v>
+      <c r="I4" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="5" spans="3:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" ht="60" spans="3:9">
       <c r="C5" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2">
         <v>0.25</v>
@@ -523,13 +1096,13 @@
         <f>(SUM(D5:G5))</f>
         <v>1</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" ht="210" spans="3:9">
+      <c r="C6" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="3:9" ht="210" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>3</v>
       </c>
       <c r="D6" s="2">
         <v>0.1</v>
@@ -537,45 +1110,46 @@
       <c r="E6" s="2">
         <v>0.1</v>
       </c>
-      <c r="F6" s="2">
-        <v>0.17</v>
+      <c r="F6" s="3">
+        <v>0.2</v>
       </c>
       <c r="G6" s="2">
         <v>0.25</v>
       </c>
       <c r="H6" s="2">
         <f t="shared" ref="H6:H7" si="0">(SUM(D6:G6))</f>
-        <v>0.62</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>13</v>
+        <v>0.65</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="7" spans="3:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" ht="45" spans="3:9">
       <c r="C7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0.08</v>
+        <v>12</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.16</v>
       </c>
       <c r="E7" s="2">
         <v>0.09</v>
       </c>
-      <c r="F7" s="2">
-        <v>0.1</v>
+      <c r="F7" s="3">
+        <v>0.2</v>
       </c>
       <c r="G7" s="2">
         <v>0.25</v>
       </c>
       <c r="H7" s="2">
         <f t="shared" si="0"/>
-        <v>0.52</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>11</v>
+        <v>0.7</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>